<commit_message>
timing - sequence diagram - etc
</commit_message>
<xml_diff>
--- a/Gantt project planner1.xlsx
+++ b/Gantt project planner1.xlsx
@@ -1484,8 +1484,8 @@
   </sheetPr>
   <dimension ref="B2:DO46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BQ26" sqref="BQ26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -2211,13 +2211,13 @@
         <v>3</v>
       </c>
       <c r="E20" s="15">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="F20" s="15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2231,13 +2231,13 @@
         <v>3</v>
       </c>
       <c r="E21" s="15">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="F21" s="15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G21" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2251,13 +2251,13 @@
         <v>5</v>
       </c>
       <c r="E22" s="15">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="F22" s="15">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G22" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2271,13 +2271,13 @@
         <v>7</v>
       </c>
       <c r="E23" s="15">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="F23" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2291,13 +2291,13 @@
         <v>4</v>
       </c>
       <c r="E24" s="15">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="F24" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2311,13 +2311,13 @@
         <v>4</v>
       </c>
       <c r="E25" s="15">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="F25" s="15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G25" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2331,13 +2331,13 @@
         <v>4</v>
       </c>
       <c r="E26" s="15">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="F26" s="15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G26" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -2351,13 +2351,13 @@
         <v>3</v>
       </c>
       <c r="E27" s="15">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="F27" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="18.95" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>